<commit_message>
fix: Suspend and update refactor
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/CaseWorkerUserXlsxWithNoPassword.xlsx
+++ b/src/integrationTest/resources/CaseWorkerUserXlsxWithNoPassword.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/350950/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA115F82-4315-D64F-B83D-78F045F69887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B8B0F0-6B53-9941-B04B-56C94F70B5C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Worker Data" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="1177">
   <si>
     <t>Region</t>
   </si>
@@ -3586,6 +3586,9 @@
   </si>
   <si>
     <t>caseworker-iac</t>
+  </si>
+  <si>
+    <t>test@justice.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -4219,7 +4222,7 @@
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4338,15 +4341,14 @@
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>9857su</v>
+        <v>3920ob</v>
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>2695fm</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f ca="1">CONCATENATE(A2,".",B2,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>9857su.2695fm861368@justice.gov.uk</v>
+        <v>8306sc</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1176</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -4408,7 +4410,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="test@justice.gov.uk" xr:uid="{DAE32429-4359-4782-88AE-2259C3A378A8}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{DAE32429-4359-4782-88AE-2259C3A378A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Refactor: validation framework refactor for Profile childs(Roles/AreaofWk/Locations) & Skip empty excel rows.
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/CaseWorkerUserXlsxWithNoPassword.xlsx
+++ b/src/integrationTest/resources/CaseWorkerUserXlsxWithNoPassword.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/350950/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B8B0F0-6B53-9941-B04B-56C94F70B5C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50717451-6A26-9E41-A51B-2EB8AC4A6110}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="1177">
   <si>
     <t>Region</t>
   </si>
@@ -4221,8 +4221,8 @@
   </sheetPr>
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4235,7 +4235,7 @@
     <col min="9" max="9" width="32.1640625" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="25.5" customWidth="1"/>
-    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="12" max="12" width="43" customWidth="1"/>
     <col min="13" max="14" width="24" customWidth="1"/>
     <col min="15" max="16" width="21.33203125" customWidth="1"/>
     <col min="17" max="20" width="19.1640625" customWidth="1"/>
@@ -4341,11 +4341,11 @@
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>3920ob</v>
+        <v>3553yb</v>
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>8306sc</v>
+        <v>2557on</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1176</v>
@@ -4377,9 +4377,7 @@
       <c r="K2" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>410</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>